<commit_message>
Updated project details and functionality
</commit_message>
<xml_diff>
--- a/testData/OpenCart_RegisterData.xlsx
+++ b/testData/OpenCart_RegisterData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>firstname</t>
   </si>
@@ -37,9 +37,6 @@
     <t>confirm password</t>
   </si>
   <si>
-    <t>testRes</t>
-  </si>
-  <si>
     <t>Ahmed</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
   </si>
   <si>
     <t>test1@gmail.com</t>
-  </si>
-  <si>
-    <t>invalid</t>
   </si>
   <si>
     <t>dkgk</t>
@@ -418,10 +412,13 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="21" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -442,19 +439,16 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
       <c r="D2">
         <v>123456</v>
@@ -464,21 +458,18 @@
       </c>
       <c r="F2">
         <v>12345</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
       <c r="D3">
         <v>123456</v>
       </c>
@@ -487,21 +478,18 @@
       </c>
       <c r="F3">
         <v>123456</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
       <c r="D4">
         <v>123456</v>
       </c>
@@ -510,21 +498,18 @@
       </c>
       <c r="F4">
         <v>123456</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
       <c r="D5">
         <v>123456</v>
       </c>
@@ -533,9 +518,6 @@
       </c>
       <c r="F5">
         <v>123456</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>